<commit_message>
dr48 - Interrum update
Updates to JSON - more logging, added a memory file for the user inputs to decrease amount of user inputs, added two new notebooks for file movement and creating creating the json
</commit_message>
<xml_diff>
--- a/seronetTemplates/dictionary/Facetdict.xlsx
+++ b/seronetTemplates/dictionary/Facetdict.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liualg/Documents/GitHub/SeroNet/seronetTemplates/dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69128330-22DA-6E43-8F30-2AB7BBDD07DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4D523F-BA7D-2C47-8C74-6C6FDBEE7C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16120" yWindow="500" windowWidth="19720" windowHeight="20200" xr2:uid="{5610A810-D1C2-A345-ADCE-1FBB1FD85AA2}"/>
   </bookViews>
@@ -267,7 +267,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -555,7 +555,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -566,7 +566,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -760,11 +760,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A23">
+    <cfRule type="duplicateValues" dxfId="1" priority="7"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B2:B23">
-    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A23">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>